<commit_message>
q1 and q2 are done
</commit_message>
<xml_diff>
--- a/2/instruction files/a2q2/A2Q2Calculations.xlsx
+++ b/2/instruction files/a2q2/A2Q2Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://saskpolytech-my.sharepoint.com/personal/grzesinam_saskpolytech_ca/Documents/MATH282archive/2025Aug/2025a2/a2q2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MATH\MATH-280\2\instruction files\a2q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FB99EAE7-A7B0-4DDA-9D63-4D1A52C32C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FFE6024-4DCB-4749-9D38-F6849EED8227}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B88CCFE-48FD-4429-9750-2254BB7C6151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3645" yWindow="3060" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="1" r:id="rId1"/>
@@ -319,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>Student Name(s):</t>
   </si>
@@ -484,12 +484,78 @@
   <si>
     <t>Fall 2025</t>
   </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>distance from 1 to 9</t>
+  </si>
+  <si>
+    <t>f(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> f(9)</t>
+  </si>
+  <si>
+    <t>distance from 1 to 5</t>
+  </si>
+  <si>
+    <t>distance from 5 to 9</t>
+  </si>
+  <si>
+    <t>f(3)</t>
+  </si>
+  <si>
+    <t>f(7)</t>
+  </si>
+  <si>
+    <t>distance from 1 to 3</t>
+  </si>
+  <si>
+    <t>distance from 3 to 5</t>
+  </si>
+  <si>
+    <t>distance from 5 to 7</t>
+  </si>
+  <si>
+    <t>distance from 7 to 9</t>
+  </si>
+  <si>
+    <t>f(9)</t>
+  </si>
+  <si>
+    <t>f(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> f(1)</t>
+  </si>
+  <si>
+    <t>f(2)</t>
+  </si>
+  <si>
+    <t>f(4)</t>
+  </si>
+  <si>
+    <t>f(6)</t>
+  </si>
+  <si>
+    <t>f(8)</t>
+  </si>
+  <si>
+    <t>Because each width is 1, we omit these cells from this table</t>
+  </si>
+  <si>
+    <t>Tie Wang</t>
+  </si>
+  <si>
+    <t>wang9431</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,6 +618,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -606,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -634,6 +706,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,6 +787,79 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4E1CBA1-FD0F-4FE8-973F-9E2460D0ACC4}" name="Table1" displayName="Table1" ref="A5:D6" totalsRowShown="0">
+  <autoFilter ref="A5:D6" xr:uid="{C4E1CBA1-FD0F-4FE8-973F-9E2460D0ACC4}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{61697732-9599-487F-BA8B-6AF9EE2BE572}" name="f(1)"/>
+    <tableColumn id="2" xr3:uid="{4B7DFE2B-23FF-4271-874A-5D4633285D8A}" name="f(9)"/>
+    <tableColumn id="3" xr3:uid="{CFCC9322-16E5-4CC1-BA5F-F2F04B26EBD6}" name="distance from 1 to 9"/>
+    <tableColumn id="4" xr3:uid="{2BAAB949-76F2-460C-8087-5E8109C7EA9E}" name="area">
+      <calculatedColumnFormula>(A6 + B6) * C6 / 2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5FB2C4ED-0AA4-4DE0-8761-44B8854C780A}" name="Table13" displayName="Table13" ref="A5:F6" totalsRowShown="0">
+  <autoFilter ref="A5:F6" xr:uid="{5FB2C4ED-0AA4-4DE0-8761-44B8854C780A}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{4EBF3C06-FCEA-4BD5-A30C-E19EFFBC9781}" name=" f(1)"/>
+    <tableColumn id="5" xr3:uid="{72B281A7-5790-4601-BDD6-FEAC1ADF766A}" name="f(5)"/>
+    <tableColumn id="2" xr3:uid="{6193B7FF-6D12-47FE-9FCD-C9DA71957EAD}" name=" f(9)"/>
+    <tableColumn id="3" xr3:uid="{DA45F128-B248-45D8-9748-500719BA7AF0}" name="distance from 1 to 5"/>
+    <tableColumn id="6" xr3:uid="{912204C4-D596-4A26-90D9-857855D91CB3}" name="distance from 5 to 9"/>
+    <tableColumn id="4" xr3:uid="{D877FE02-D5CF-47FA-927D-1BEC4668E56F}" name="area">
+      <calculatedColumnFormula>(A6 + B6) * D6 / 2  +(B6 + C6) * E6 / 2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A8E0A1D9-A538-4B99-AA61-7D7D663BC97C}" name="Table134" displayName="Table134" ref="A4:J5" totalsRowShown="0">
+  <autoFilter ref="A4:J5" xr:uid="{A8E0A1D9-A538-4B99-AA61-7D7D663BC97C}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{7BA1C46F-0A6F-4B80-96F7-9C755FEC0B0A}" name=" f(1)"/>
+    <tableColumn id="7" xr3:uid="{A82A52A4-AE31-42EA-93EB-1C82B0D5F6A2}" name="f(3)"/>
+    <tableColumn id="5" xr3:uid="{E347E93C-CB0B-4039-936E-64684E75F847}" name="f(5)"/>
+    <tableColumn id="8" xr3:uid="{FFF37427-DA55-4F01-A56D-BA5D564C86FF}" name="f(7)"/>
+    <tableColumn id="2" xr3:uid="{1C5D62A0-E31C-4CE5-A33F-B4FCBD780FDC}" name=" f(9)"/>
+    <tableColumn id="3" xr3:uid="{1330739F-AA5A-400D-8422-4D26A44F461F}" name="distance from 1 to 3"/>
+    <tableColumn id="6" xr3:uid="{F861C881-0127-48D6-8901-EB31FB98CC37}" name="distance from 3 to 5"/>
+    <tableColumn id="9" xr3:uid="{F30D1D07-D262-4374-B943-5BDC383F9F39}" name="distance from 5 to 7"/>
+    <tableColumn id="10" xr3:uid="{5F8454E5-2C2C-47A2-87E0-EB4BC9EAECBE}" name="distance from 7 to 9"/>
+    <tableColumn id="4" xr3:uid="{775A62CC-3DE4-46CE-BEAF-BAA7ED0D3307}" name="area">
+      <calculatedColumnFormula>(A5 + B5) * F5 / 2  +(B5 + C5) * G5 / 2 + (C5 + D5) * H5 / 2 +(D5 + E5) * G5 / 2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A11C898A-A5D7-4D82-A75C-3966A7950EDE}" name="Table1345" displayName="Table1345" ref="A5:I6" totalsRowShown="0">
+  <autoFilter ref="A5:I6" xr:uid="{A11C898A-A5D7-4D82-A75C-3966A7950EDE}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{82DD2AED-7174-4185-B8CD-14C2249F02FA}" name=" f(1)"/>
+    <tableColumn id="11" xr3:uid="{E68DA61E-9590-425D-B4F9-751B42D6078E}" name="f(2)"/>
+    <tableColumn id="7" xr3:uid="{EC12FE53-1100-4ECB-8083-CDACF3E18213}" name="f(3)"/>
+    <tableColumn id="12" xr3:uid="{4AF4A317-7723-46FB-932B-42669ECBE469}" name="f(4)"/>
+    <tableColumn id="5" xr3:uid="{1D51A828-83ED-4B7F-800A-2A4ED0B6E588}" name="f(5)"/>
+    <tableColumn id="13" xr3:uid="{142C30AB-9CDE-4061-A88A-3318811296D1}" name="f(6)"/>
+    <tableColumn id="8" xr3:uid="{AAE829FF-E1F3-4DF7-9689-3E57E76339BF}" name="f(7)"/>
+    <tableColumn id="14" xr3:uid="{C621D51C-50B9-49FF-8DDD-C0AC7BEFAFD8}" name="f(8)"/>
+    <tableColumn id="4" xr3:uid="{C2818073-9005-4CBA-8BC9-8C169A79DBA0}" name="area">
+      <calculatedColumnFormula>A6*1 + B6*1 + C6*1  + D6*1  + E6*1 + F6*1 + G6*1 + H6*1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1003,31 +1152,35 @@
   <dimension ref="B2:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1035,7 +1188,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1043,7 +1196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1051,7 +1204,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -1059,10 +1212,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1070,7 +1223,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1078,7 +1231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1086,25 +1239,27 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C16" s="11"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="11"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="11"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="11"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C20" s="9"/>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="9">
+        <v>16.987752593558898</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1119,121 +1274,372 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>3.1699000000000002</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <f>(A6 + B6) * C6 / 2</f>
+        <v>12.679600000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="5" width="24" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="B3" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>2.3218999999999999</v>
+      </c>
+      <c r="C6">
+        <v>3.1699000000000002</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <f>(A6 + B6) * D6 / 2  +(B6 + C6) * E6 / 2</f>
+        <v>15.627399999999998</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1.5849</v>
+      </c>
+      <c r="C5">
+        <v>2.3218999999999999</v>
+      </c>
+      <c r="D5">
+        <v>2.8073000000000001</v>
+      </c>
+      <c r="E5">
+        <v>3.1699000000000002</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f>(A5 + B5) * F5 / 2  +(B5 + C5) * G5 / 2 + (C5 + D5) * H5 / 2 +(D5 + E5) * G5 / 2</f>
+        <v>16.598099999999999</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1.5849</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2.3218999999999999</v>
+      </c>
+      <c r="F6">
+        <v>2.5849000000000002</v>
+      </c>
+      <c r="G6">
+        <v>2.8073000000000001</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <f>A6*1 + B6*1 + C6*1  + D6*1  + E6*1 + F6*1 + G6*1 + H6*1</f>
+        <v>15.299000000000001</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:I4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1242,16 +1648,16 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
@@ -1259,15 +1665,15 @@
       <c r="C1" s="12"/>
       <c r="D1" s="10">
         <f>Documentation!C20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16.987752593558898</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1281,53 +1687,87 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="9">
+        <v>12.679600000000001</v>
+      </c>
+      <c r="C5" s="9">
+        <f>D1-B5</f>
+        <v>4.3081525935588978</v>
+      </c>
+      <c r="D5" s="14">
+        <f>C5/D1</f>
+        <v>0.25360344576670979</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="9">
+        <v>15.627399999999998</v>
+      </c>
+      <c r="C6" s="9">
+        <f>D1-B6</f>
+        <v>1.3603525935589005</v>
+      </c>
+      <c r="D6" s="14">
+        <f>C6/D1</f>
+        <v>8.0078432156746496E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="9">
+        <v>16.598099999999999</v>
+      </c>
+      <c r="C7" s="9">
+        <f>D1-B7</f>
+        <v>0.3896525935588997</v>
+      </c>
+      <c r="D7" s="14">
+        <f>C7/D1</f>
+        <v>2.2937265621977621E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="9">
+        <v>15.299000000000001</v>
+      </c>
+      <c r="C8" s="9">
+        <f>D1-B8</f>
+        <v>1.6887525935588972</v>
+      </c>
+      <c r="D8" s="14">
+        <f>C8/D1</f>
+        <v>9.9410006371249318E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="9">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1340,6 +1780,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2c703f2b-2e45-4897-8afb-57fd36e2d636">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="906ba92d-599e-4b69-b48c-622f8dfa89d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B4FC342DA62764FBC3EF9308002E92D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90704c012a057dc0ea95fb8870db3e5d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c703f2b-2e45-4897-8afb-57fd36e2d636" xmlns:ns3="906ba92d-599e-4b69-b48c-622f8dfa89d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4369950507baaa2fd07ca04966e39d1" ns2:_="" ns3:_="">
     <xsd:import namespace="2c703f2b-2e45-4897-8afb-57fd36e2d636"/>
@@ -1574,43 +2034,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2c703f2b-2e45-4897-8afb-57fd36e2d636">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="906ba92d-599e-4b69-b48c-622f8dfa89d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03389DFB-5033-4979-B9BF-40B1C40DF65A}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1794B95D-BEAC-42BE-896B-D7F814C1A91B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2c703f2b-2e45-4897-8afb-57fd36e2d636"/>
+    <ds:schemaRef ds:uri="906ba92d-599e-4b69-b48c-622f8dfa89d0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79630B1B-232B-4EEC-B212-947320836E0D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03389DFB-5033-4979-B9BF-40B1C40DF65A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2c703f2b-2e45-4897-8afb-57fd36e2d636"/>
+    <ds:schemaRef ds:uri="906ba92d-599e-4b69-b48c-622f8dfa89d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>